<commit_message>
get journal names from csv and get pmcid of 125 journals
</commit_message>
<xml_diff>
--- a/journal-list.xlsx
+++ b/journal-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V119736\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andtr/Documents/CV/JournalCollector2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DD3E2B-9608-4EA7-95D7-5470C7FBD322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3CE231-B44E-1749-B0B2-C9151A8A1A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nursing Journals" sheetId="1" r:id="rId1"/>
@@ -6731,20 +6731,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="47.33203125" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13.25" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.25" customWidth="1"/>
-    <col min="10" max="10" width="12.25" customWidth="1"/>
-    <col min="11" max="11" width="47.08203125" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" customWidth="1"/>
+    <col min="11" max="11" width="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -11797,7 +11797,7 @@
     <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;KEEDC00 RMIT Classification: Trusted&amp;1#_x000D_</oddHeader>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:J2 A5:J5 B3:J3 B4:J4 B38:J38 B6:J6 B7:J7 B8:J8 B9:J9 B10:J10 B11:J11 B12:J12 B13:J13 B14:J14 B15:J15 B16:J16 B17:J17 B18:J18 B19:J19 B20:J20 B21:J21 B22:J22 B23:J23 B24:J24 B25:J25 B26:J26 B27:J27 B28:J28 B29:J29 B30:J30 B31:J31 B32:J32 B33:J33 B34:J34 B35:J35 B36:J36 B37:J37 B77:J77 B39:J39 B40:J40 B41:J41 B42:J42 B43:J43 B44:J44 B45:J45 B46:J46 B47:J47 B48:J48 B49:J49 B50:J50 B51:J51 B52:J52 B53:J53 B54:J54 B55:J55 B56:J56 B57:J57 B58:J58 B59:J59 B60:J60 B61:J61 B62:J62 B63:J63 B64:J64 B65:J65 B66:J66 B67:J67 B68:J68 B69:J69 B70:J70 B71:J71 B72:J72 B73:J73 B74:J74 B75:J75 B76:J76 B81:J81 B78:J78 B79:J79 B80:J80 B127:J127 B82:J82 B83:J83 B84:J84 B85:J85 B86:J86 B87:J87 B88:J88 B89:J89 B90:J90 B91:J91 B92:J92 B93:J93 B94:J94 B95:J95 B96:J96 B97:J97 B98:J98 B99:J99 B100:J100 B101:J101 B102:J102 B103:J103 B104:J104 B105:J105 B106:J106 B107:J107 B108:J108 B109:J109 B110:J110 B111:J111 B112:J112 B113:J113 B114:J114 B115:J115 B116:J116 B117:J117 B118:J118 B119:J119 B120:J120 B121:J121 B122:J122 B123:J123 B124:J124 B125:J125 B126:J126 B128:J129" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:J1 A5:J5 B3:J3 B4:J4 B38:J38 B6:J6 B7:J7 B8:J8 C9:J9 B10:J10 B11:J11 B12:J12 B13:J13 B14:J14 B15:J15 B16:J16 B17:J17 B18:J18 B19:J19 B20:J20 B21:J21 B22:J22 B23:J23 B24:J24 B25:J25 B26:J26 B27:J27 B28:J28 B29:J29 B30:J30 B31:J31 B32:J32 B33:J33 B34:J34 B35:J35 B36:J36 B37:J37 B77:J77 B39:J39 B40:J40 B41:J41 B42:J42 B43:J43 B44:J44 B45:J45 B46:J46 B47:J47 B48:J48 B49:J49 B50:J50 B51:J51 B52:J52 B53:J53 B54:J54 B55:J55 B56:J56 B57:J57 B58:J58 B59:J59 B60:J60 B61:J61 B62:J62 B63:J63 B64:J64 B65:J65 B66:J66 B67:J67 B68:J68 B69:J69 B70:J70 B71:J71 B72:J72 B73:J73 B74:J74 B75:J75 B76:J76 B81:J81 B78:J78 B79:J79 B80:J80 B127:J127 B82:J82 B83:J83 B84:J84 B85:J85 B86:J86 B87:J87 B88:J88 B89:J89 B90:J90 B91:J91 B92:J92 B93:J93 B94:J94 B95:J95 B96:J96 B97:J97 B98:J98 B99:J99 B100:J100 B101:J101 B102:J102 B103:J103 B104:J104 B105:J105 B106:J106 B107:J107 B108:J108 B109:J109 B110:J110 B111:J111 B112:J112 B113:J113 B114:J114 B115:J115 B116:J116 B117:J117 B118:J118 B119:J119 B120:J120 B121:J121 B122:J122 B123:J123 B124:J124 B125:J125 B126:J126 B128:J129 C2:J2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -11811,21 +11811,21 @@
       <selection pane="bottomLeft" activeCell="N175" sqref="N175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="49.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.08203125" style="4" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="9.25" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.58203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.75" style="4" customWidth="1"/>
+    <col min="2" max="2" width="22" style="4" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.58203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="5.5" style="4" customWidth="1"/>
     <col min="9" max="9" width="8" style="4" customWidth="1"/>
     <col min="10" max="10" width="9" style="4" customWidth="1"/>
-    <col min="11" max="11" width="28.75" style="4" customWidth="1"/>
+    <col min="11" max="11" width="28.6640625" style="4" customWidth="1"/>
     <col min="12" max="12" width="14.5" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="8.58203125" style="4"/>
+    <col min="13" max="16384" width="8.5" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -12727,7 +12727,7 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="16">
+    <row r="23" spans="1:13">
       <c r="A23" s="4" t="s">
         <v>1159</v>
       </c>

</xml_diff>